<commit_message>
Updating Excel examples to handle rdfs:comment in 4 languages
</commit_message>
<xml_diff>
--- a/testdata/Properties.xlsx
+++ b/testdata/Properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ritagautschy/Documents/Ontologien/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrivoal/Git-projets/medialitterature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FCE124-D34B-FA49-A5DE-60DA442D292B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B05C1F0-00BF-A041-B1F2-B0672A71AD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="7320" windowWidth="24580" windowHeight="12560" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
+    <workbookView xWindow="15420" yWindow="4640" windowWidth="35780" windowHeight="23420" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="186">
   <si>
     <t>super</t>
   </si>
@@ -258,250 +258,331 @@
     <t>fr</t>
   </si>
   <si>
+    <t>owner of</t>
+  </si>
+  <si>
+    <t>anthroponym</t>
+  </si>
+  <si>
+    <t>generic anthroponym</t>
+  </si>
+  <si>
+    <t>designated as</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>related with</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>birth date</t>
+  </si>
+  <si>
+    <t>death date</t>
+  </si>
+  <si>
+    <t>bibliography</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>corresponds to generic anthroponym</t>
+  </si>
+  <si>
+    <t>TM name identifier</t>
+  </si>
+  <si>
+    <t>Egyptian name</t>
+  </si>
+  <si>
+    <t>Greek name</t>
+  </si>
+  <si>
+    <t>Latin name</t>
+  </si>
+  <si>
+    <t>Coptic name</t>
+  </si>
+  <si>
+    <t>other name variant</t>
+  </si>
+  <si>
+    <t>linguistic origin</t>
+  </si>
+  <si>
+    <t>English translation</t>
+  </si>
+  <si>
+    <t>French translation</t>
+  </si>
+  <si>
+    <t>German translation</t>
+  </si>
+  <si>
+    <t>family relation</t>
+  </si>
+  <si>
+    <t>related to</t>
+  </si>
+  <si>
+    <t>terminus post quem</t>
+  </si>
+  <si>
+    <t>terminus ante quem</t>
+  </si>
+  <si>
+    <t>most common in</t>
+  </si>
+  <si>
+    <t>most widespread in</t>
+  </si>
+  <si>
+    <t>related to god</t>
+  </si>
+  <si>
+    <t>related to place</t>
+  </si>
+  <si>
+    <t>attested amount</t>
+  </si>
+  <si>
+    <t>has alias</t>
+  </si>
+  <si>
+    <t>is alias</t>
+  </si>
+  <si>
+    <t>is alais of</t>
+  </si>
+  <si>
+    <t>has title</t>
+  </si>
+  <si>
+    <t>English title</t>
+  </si>
+  <si>
+    <t>French title</t>
+  </si>
+  <si>
+    <t>German title</t>
+  </si>
+  <si>
+    <t>is equivalent to</t>
+  </si>
+  <si>
+    <t>occupation field</t>
+  </si>
+  <si>
+    <t>Anthroponyme</t>
+  </si>
+  <si>
+    <t>Propriétaire de</t>
+  </si>
+  <si>
+    <t>correspond à l'anthroponyme générique</t>
+  </si>
+  <si>
+    <t>a un alias</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>désigné sous le nom de</t>
+  </si>
+  <si>
+    <t>a un titre</t>
+  </si>
+  <si>
+    <t>statut</t>
+  </si>
+  <si>
+    <t>en rapport avec</t>
+  </si>
+  <si>
+    <t>Âge</t>
+  </si>
+  <si>
+    <t>Date de naissance</t>
+  </si>
+  <si>
+    <t>Date du décès</t>
+  </si>
+  <si>
+    <t>Littérature</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
+  </si>
+  <si>
+    <t>connecté avec</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Anthroponyme générique</t>
+  </si>
+  <si>
+    <t>Identifiant du nom de la MT</t>
+  </si>
+  <si>
+    <t>Nom égyptien</t>
+  </si>
+  <si>
+    <t>Nom grec</t>
+  </si>
+  <si>
+    <t>Nom latin</t>
+  </si>
+  <si>
+    <t>Nom copte</t>
+  </si>
+  <si>
+    <t>Autre variante du nom</t>
+  </si>
+  <si>
+    <t>origine linguistique</t>
+  </si>
+  <si>
+    <t>Traduction en anglais</t>
+  </si>
+  <si>
+    <t>Traduction en français</t>
+  </si>
+  <si>
+    <t>Traduction en allemand</t>
+  </si>
+  <si>
+    <t>associé à une divinité</t>
+  </si>
+  <si>
+    <t>associé à un lieu</t>
+  </si>
+  <si>
+    <t>Nombre de références</t>
+  </si>
+  <si>
+    <t>le plus courant dans</t>
+  </si>
+  <si>
+    <t>est un alias</t>
+  </si>
+  <si>
+    <t>est un alias de</t>
+  </si>
+  <si>
+    <t>titre</t>
+  </si>
+  <si>
+    <t>Titre anglais</t>
+  </si>
+  <si>
+    <t>Titre français</t>
+  </si>
+  <si>
+    <t>Titre allemand</t>
+  </si>
+  <si>
+    <t>est équivalent à</t>
+  </si>
+  <si>
+    <t>Domaine d'emploi</t>
+  </si>
+  <si>
+    <t>comment_fr</t>
+  </si>
+  <si>
+    <t>comment_en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A strange chance put me in possession of this journal.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I had established myself for several months in a central city in one of our southern departments, whose shore is bathed by the Mediterranean, and I was desirous of purchasing a country place in that marvellously picturesque land. </t>
+  </si>
+  <si>
+    <t>I had already looked at several pieces of property when, one day, the notary, who had been giving me some necessary directions for one of my explorations, said to me:</t>
+  </si>
+  <si>
+    <t>I have just received notice that at about eight leagues from here, in one of the most beautiful situations in the world, neither too far nor too near to the sea, there is a country house for sale.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I know nothing of it whatever; but if you would like to see it, monsieur, here are the precise directions how to find it. </t>
+  </si>
+  <si>
+    <t>You will have to arrange the affair with the curé of the village of ——."</t>
+  </si>
+  <si>
     <t>de</t>
   </si>
   <si>
-    <t>Anthroponym</t>
-  </si>
-  <si>
-    <t>Besitzer von</t>
-  </si>
-  <si>
-    <t>owner of</t>
-  </si>
-  <si>
-    <t>anthroponym</t>
-  </si>
-  <si>
-    <t>generic anthroponym</t>
-  </si>
-  <si>
-    <t>Generisches Anthroponym</t>
-  </si>
-  <si>
-    <t>Geschlecht</t>
-  </si>
-  <si>
-    <t>bezeichnet als</t>
-  </si>
-  <si>
-    <t>designated as</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>Titel</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>verwandt mit</t>
-  </si>
-  <si>
-    <t>related with</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>Alter</t>
-  </si>
-  <si>
-    <t>birth date</t>
-  </si>
-  <si>
-    <t>Geburtsdatum</t>
-  </si>
-  <si>
-    <t>death date</t>
-  </si>
-  <si>
-    <t>Sterbedatum</t>
-  </si>
-  <si>
-    <t>bibliography</t>
-  </si>
-  <si>
-    <t>Literatur</t>
-  </si>
-  <si>
-    <t>remark</t>
-  </si>
-  <si>
-    <t>Bemerkung</t>
-  </si>
-  <si>
-    <t>entspricht generischem Anthroponym</t>
-  </si>
-  <si>
-    <t>corresponds to generic anthroponym</t>
-  </si>
-  <si>
-    <t>TM name identifier</t>
-  </si>
-  <si>
-    <t>TM-Namensidentifikator</t>
-  </si>
-  <si>
-    <t>ägyptischer Name</t>
-  </si>
-  <si>
-    <t>griechischer Name</t>
-  </si>
-  <si>
-    <t>lateinischer Name</t>
-  </si>
-  <si>
-    <t>Egyptian name</t>
-  </si>
-  <si>
-    <t>Greek name</t>
-  </si>
-  <si>
-    <t>Latin name</t>
-  </si>
-  <si>
-    <t>Coptic name</t>
-  </si>
-  <si>
-    <t>Andere Namensvariante</t>
-  </si>
-  <si>
-    <t>koptischer Name</t>
-  </si>
-  <si>
-    <t>other name variant</t>
-  </si>
-  <si>
-    <t>linguistic origin</t>
-  </si>
-  <si>
-    <t>sprachlicher Ursprung</t>
-  </si>
-  <si>
-    <t>English translation</t>
-  </si>
-  <si>
-    <t>French translation</t>
-  </si>
-  <si>
-    <t>German translation</t>
-  </si>
-  <si>
-    <t>englische Übersetzung</t>
-  </si>
-  <si>
-    <t>französische Übersetzung</t>
-  </si>
-  <si>
-    <t>deutsche Übersetzung</t>
-  </si>
-  <si>
-    <t>Verwandtschaftsbeziehung</t>
-  </si>
-  <si>
-    <t>family relation</t>
-  </si>
-  <si>
-    <t>related to</t>
-  </si>
-  <si>
-    <t>verbunden mit</t>
-  </si>
-  <si>
-    <t>terminus post quem</t>
-  </si>
-  <si>
-    <t>terminus ante quem</t>
-  </si>
-  <si>
-    <t>most common in</t>
-  </si>
-  <si>
-    <t>am weitesten verbreitet in</t>
-  </si>
-  <si>
-    <t>most widespread in</t>
-  </si>
-  <si>
-    <t>am gebräuchlichsten in</t>
-  </si>
-  <si>
-    <t>verbunden mit Gottheit</t>
-  </si>
-  <si>
-    <t>related to god</t>
-  </si>
-  <si>
-    <t>related to place</t>
-  </si>
-  <si>
-    <t>verbunden mit Ort</t>
-  </si>
-  <si>
-    <t>attested amount</t>
-  </si>
-  <si>
-    <t>Anzahl Belegstellen</t>
-  </si>
-  <si>
     <t>it</t>
   </si>
   <si>
-    <t>has alias</t>
-  </si>
-  <si>
-    <t>hat Alias</t>
-  </si>
-  <si>
-    <t>is alias</t>
-  </si>
-  <si>
-    <t>ist Alias</t>
-  </si>
-  <si>
-    <t>is alais of</t>
-  </si>
-  <si>
-    <t>has title</t>
-  </si>
-  <si>
-    <t>hat Titel</t>
-  </si>
-  <si>
-    <t>ist Alias von</t>
-  </si>
-  <si>
-    <t>English title</t>
-  </si>
-  <si>
-    <t>French title</t>
-  </si>
-  <si>
-    <t>German title</t>
-  </si>
-  <si>
-    <t>englischer Titel</t>
-  </si>
-  <si>
-    <t>französischer Titel</t>
-  </si>
-  <si>
-    <t>deutscher Titel</t>
-  </si>
-  <si>
-    <t>is equivalent to</t>
-  </si>
-  <si>
-    <t>ist äquivalent zu</t>
-  </si>
-  <si>
-    <t>occupation field</t>
-  </si>
-  <si>
-    <t>Beschäftigungsfeld</t>
+    <t>comment_it</t>
+  </si>
+  <si>
+    <t>comment_de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein seltsamer Zufall brachte mich in den Besitz dieses Tagebuchs.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich hatte mich für einige Monate in einer Stadt im Zentrum eines unserer südlichen Departements niedergelassen, dessen Ufer vom Mittelmeer umspült wird, und wollte ein Grundstück in diesem wunderbar malerischen Land erwerben. </t>
+  </si>
+  <si>
+    <t>Ich hatte bereits mehrere Grundstücke besichtigt, als eines Tages der Notar, der mir die notwendigen Anweisungen für eine meiner Erkundungen gegeben hatte, zu mir sagte:</t>
+  </si>
+  <si>
+    <t>Ich habe soeben erfahren, dass etwa acht Meilen von hier, in einer der schönsten Lagen der Welt, weder zu weit noch zu nah am Meer, ein Landhaus zum Verkauf steht.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich weiß nichts davon, aber wenn Sie es sehen möchten, Monsieur, finden Sie hier die genaue Wegbeschreibung. </t>
+  </si>
+  <si>
+    <t>Sie werden die Angelegenheit mit dem Pfarrer des Dorfes -- regeln müssen."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un étrange hasard m'a mis en possession de ce journal.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je m'étais établi depuis plusieurs mois dans une ville centrale d'un de nos départements méridionaux, dont le rivage est baigné par la Méditerranée, et je désirais acheter une maison de campagne dans cette contrée merveilleusement pittoresque. </t>
+  </si>
+  <si>
+    <t>J'avais déjà examiné plusieurs propriétés quand, un jour, le notaire, qui me donnait des indications nécessaires pour une de mes explorations, me dit :</t>
+  </si>
+  <si>
+    <t>Je viens de recevoir avis qu'à huit lieues d'ici environ, dans une des plus belles situations du monde, ni trop loin ni trop près de la mer, il y a une maison de campagne à vendre.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je n'en sais rien du tout ; mais si vous voulez la voir, monsieur, voici les indications précises pour la trouver. </t>
+  </si>
+  <si>
+    <t>Vous devrez arranger l'affaire avec le curé du village de --."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uno strano caso mi mise in possesso di questo diario.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mi ero stabilito da diversi mesi in una città centrale di uno dei nostri dipartimenti del sud, la cui riva è bagnata dal Mediterraneo, e desideravo acquistare un posto in campagna in quella terra meravigliosamente pittoresca. </t>
+  </si>
+  <si>
+    <t>Avevo già visto diverse proprietà quando un giorno il notaio, che mi aveva dato alcune indicazioni necessarie per una delle mie esplorazioni, mi disse</t>
+  </si>
+  <si>
+    <t>Ho appena ricevuto la notizia che a circa otto leghe da qui, in una delle situazioni più belle del mondo, né troppo lontano né troppo vicino al mare, c'è una casa di campagna in vendita.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non ne so nulla; ma se volete vederla, signore, eccovi le indicazioni precise per trovarla. </t>
+  </si>
+  <si>
+    <t>Dovrete organizzare l'affare con il curato del villaggio di --".</t>
   </si>
 </sst>
 </file>
@@ -642,8 +723,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Feuil1" xfId="1" xr:uid="{62E45FE5-1366-448C-9556-6A8FC585BB6F}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -659,7 +740,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -955,11 +1036,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3015D75-1C5B-4AD1-9C97-0CD088290370}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -967,19 +1048,21 @@
     <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="24" style="16" customWidth="1"/>
-    <col min="6" max="6" width="31.83203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="23.1640625" customWidth="1"/>
-    <col min="9" max="9" width="23.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="23.1640625" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="31.33203125" style="16" customWidth="1"/>
+    <col min="6" max="7" width="24" style="16" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="31.83203125" style="16" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" style="16" customWidth="1"/>
+    <col min="11" max="11" width="31.83203125" style="16" customWidth="1"/>
+    <col min="12" max="12" width="23.1640625" customWidth="1"/>
+    <col min="13" max="13" width="23.1640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="23.1640625" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>74</v>
       </c>
@@ -993,22 +1076,34 @@
         <v>75</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>77</v>
+        <v>164</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>76</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="H1" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="L1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1019,18 +1114,31 @@
         <v>18</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="16" t="s">
         <v>78</v>
       </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
+        <v>117</v>
+      </c>
       <c r="G2" s="16"/>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" t="s">
+        <v>168</v>
+      </c>
+      <c r="J2" t="s">
+        <v>174</v>
+      </c>
+      <c r="K2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -1041,18 +1149,31 @@
         <v>21</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="G3" s="16"/>
-      <c r="H3" s="8" t="s">
+      <c r="H3" t="s">
+        <v>159</v>
+      </c>
+      <c r="I3" t="s">
+        <v>169</v>
+      </c>
+      <c r="J3" t="s">
+        <v>175</v>
+      </c>
+      <c r="K3" t="s">
+        <v>181</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -1063,18 +1184,31 @@
         <v>38</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>102</v>
+        <v>88</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16" t="s">
+        <v>119</v>
       </c>
       <c r="G4" s="16"/>
-      <c r="H4" s="8" t="s">
+      <c r="H4" t="s">
+        <v>160</v>
+      </c>
+      <c r="I4" t="s">
+        <v>170</v>
+      </c>
+      <c r="J4" t="s">
+        <v>176</v>
+      </c>
+      <c r="K4" t="s">
+        <v>182</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1085,18 +1219,31 @@
         <v>39</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>142</v>
+        <v>108</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16" t="s">
+        <v>120</v>
       </c>
       <c r="G5" s="16"/>
-      <c r="H5" s="8" t="s">
+      <c r="H5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I5" t="s">
+        <v>171</v>
+      </c>
+      <c r="J5" t="s">
+        <v>177</v>
+      </c>
+      <c r="K5" t="s">
+        <v>183</v>
+      </c>
+      <c r="L5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1109,18 +1256,31 @@
       <c r="D6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>84</v>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16" t="s">
+        <v>121</v>
       </c>
       <c r="G6" s="16"/>
-      <c r="H6" s="2" t="s">
+      <c r="H6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" t="s">
+        <v>172</v>
+      </c>
+      <c r="J6" t="s">
+        <v>178</v>
+      </c>
+      <c r="K6" t="s">
+        <v>184</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1131,20 +1291,33 @@
         <v>24</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="G7" s="16"/>
-      <c r="H7" s="7" t="s">
+      <c r="H7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" t="s">
+        <v>173</v>
+      </c>
+      <c r="J7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K7" t="s">
+        <v>185</v>
+      </c>
+      <c r="L7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="M7" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1155,18 +1328,31 @@
         <v>40</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>147</v>
+        <v>111</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16" t="s">
+        <v>123</v>
       </c>
       <c r="G8" s="16"/>
-      <c r="H8" s="8" t="s">
+      <c r="H8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I8" t="s">
+        <v>168</v>
+      </c>
+      <c r="J8" t="s">
+        <v>174</v>
+      </c>
+      <c r="K8" t="s">
+        <v>180</v>
+      </c>
+      <c r="L8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1179,18 +1365,31 @@
       <c r="D9" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>89</v>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="G9" s="16"/>
-      <c r="H9" s="7" t="s">
+      <c r="H9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I9" t="s">
+        <v>169</v>
+      </c>
+      <c r="J9" t="s">
+        <v>175</v>
+      </c>
+      <c r="K9" t="s">
+        <v>181</v>
+      </c>
+      <c r="L9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="M9" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1201,18 +1400,31 @@
         <v>41</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>90</v>
+        <v>82</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16" t="s">
+        <v>125</v>
       </c>
       <c r="G10" s="16"/>
-      <c r="H10" s="8" t="s">
+      <c r="H10" t="s">
+        <v>160</v>
+      </c>
+      <c r="I10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J10" t="s">
+        <v>176</v>
+      </c>
+      <c r="K10" t="s">
+        <v>182</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1223,18 +1435,31 @@
         <v>29</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>93</v>
+        <v>83</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="G11" s="16"/>
-      <c r="H11" s="7" t="s">
+      <c r="H11" t="s">
+        <v>161</v>
+      </c>
+      <c r="I11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1245,16 +1470,28 @@
         <v>30</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="H12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" t="s">
+        <v>162</v>
+      </c>
+      <c r="I12" t="s">
+        <v>172</v>
+      </c>
+      <c r="J12" t="s">
+        <v>178</v>
+      </c>
+      <c r="K12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L12" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1265,16 +1502,28 @@
         <v>30</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="H13" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" t="s">
+        <v>163</v>
+      </c>
+      <c r="I13" t="s">
+        <v>173</v>
+      </c>
+      <c r="J13" t="s">
+        <v>179</v>
+      </c>
+      <c r="K13" t="s">
+        <v>185</v>
+      </c>
+      <c r="L13" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -1285,16 +1534,28 @@
         <v>32</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="H14" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H14" t="s">
+        <v>158</v>
+      </c>
+      <c r="I14" t="s">
+        <v>168</v>
+      </c>
+      <c r="J14" t="s">
+        <v>174</v>
+      </c>
+      <c r="K14" t="s">
+        <v>180</v>
+      </c>
+      <c r="L14" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1305,16 +1566,28 @@
         <v>18</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="H15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="H15" t="s">
+        <v>159</v>
+      </c>
+      <c r="I15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J15" t="s">
+        <v>175</v>
+      </c>
+      <c r="K15" t="s">
+        <v>181</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>34</v>
       </c>
@@ -1325,17 +1598,29 @@
         <v>35</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="H16" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="H16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J16" t="s">
+        <v>176</v>
+      </c>
+      <c r="K16" t="s">
+        <v>182</v>
+      </c>
+      <c r="L16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -1346,19 +1631,31 @@
         <v>24</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="H17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="H17" t="s">
+        <v>161</v>
+      </c>
+      <c r="I17" t="s">
+        <v>171</v>
+      </c>
+      <c r="J17" t="s">
+        <v>177</v>
+      </c>
+      <c r="K17" t="s">
+        <v>183</v>
+      </c>
+      <c r="L17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="M17" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
@@ -1369,18 +1666,31 @@
         <v>18</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16" t="s">
+        <v>133</v>
       </c>
       <c r="G18" s="16"/>
-      <c r="H18" s="4" t="s">
+      <c r="H18" t="s">
+        <v>162</v>
+      </c>
+      <c r="I18" t="s">
+        <v>172</v>
+      </c>
+      <c r="J18" t="s">
+        <v>178</v>
+      </c>
+      <c r="K18" t="s">
+        <v>184</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1391,17 +1701,29 @@
         <v>29</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="H19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" t="s">
+        <v>163</v>
+      </c>
+      <c r="I19" t="s">
+        <v>173</v>
+      </c>
+      <c r="J19" t="s">
+        <v>179</v>
+      </c>
+      <c r="K19" t="s">
+        <v>185</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1412,17 +1734,29 @@
         <v>18</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>106</v>
+        <v>90</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>135</v>
       </c>
       <c r="H20" t="s">
+        <v>158</v>
+      </c>
+      <c r="I20" t="s">
+        <v>168</v>
+      </c>
+      <c r="J20" t="s">
+        <v>174</v>
+      </c>
+      <c r="K20" t="s">
+        <v>180</v>
+      </c>
+      <c r="L20" t="s">
         <v>19</v>
       </c>
-      <c r="I20"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M20"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1433,17 +1767,29 @@
         <v>18</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>107</v>
+        <v>91</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>136</v>
       </c>
       <c r="H21" t="s">
+        <v>159</v>
+      </c>
+      <c r="I21" t="s">
+        <v>169</v>
+      </c>
+      <c r="J21" t="s">
+        <v>175</v>
+      </c>
+      <c r="K21" t="s">
+        <v>181</v>
+      </c>
+      <c r="L21" t="s">
         <v>19</v>
       </c>
-      <c r="I21"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M21"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1454,17 +1800,29 @@
         <v>18</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="H22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" t="s">
+        <v>160</v>
+      </c>
+      <c r="I22" t="s">
+        <v>170</v>
+      </c>
+      <c r="J22" t="s">
+        <v>176</v>
+      </c>
+      <c r="K22" t="s">
+        <v>182</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I22"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M22"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1475,17 +1833,29 @@
         <v>18</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>114</v>
+        <v>93</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>138</v>
       </c>
       <c r="H23" t="s">
+        <v>161</v>
+      </c>
+      <c r="I23" t="s">
+        <v>171</v>
+      </c>
+      <c r="J23" t="s">
+        <v>177</v>
+      </c>
+      <c r="K23" t="s">
+        <v>183</v>
+      </c>
+      <c r="L23" t="s">
         <v>19</v>
       </c>
-      <c r="I23"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M23"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1496,17 +1866,29 @@
         <v>18</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="H24" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" t="s">
+        <v>162</v>
+      </c>
+      <c r="I24" t="s">
+        <v>172</v>
+      </c>
+      <c r="J24" t="s">
+        <v>178</v>
+      </c>
+      <c r="K24" t="s">
+        <v>184</v>
+      </c>
+      <c r="L24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I24"/>
-    </row>
-    <row r="25" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M24"/>
+    </row>
+    <row r="25" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
@@ -1517,20 +1899,33 @@
         <v>24</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>117</v>
+        <v>95</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="G25" s="16"/>
-      <c r="H25" s="2" t="s">
+      <c r="H25" t="s">
+        <v>163</v>
+      </c>
+      <c r="I25" t="s">
+        <v>173</v>
+      </c>
+      <c r="J25" t="s">
+        <v>179</v>
+      </c>
+      <c r="K25" t="s">
+        <v>185</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="M25" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>51</v>
       </c>
@@ -1541,19 +1936,32 @@
         <v>18</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>121</v>
+        <v>96</v>
+      </c>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="G26" s="16"/>
-      <c r="H26" s="4" t="s">
+      <c r="H26" t="s">
+        <v>158</v>
+      </c>
+      <c r="I26" t="s">
+        <v>168</v>
+      </c>
+      <c r="J26" t="s">
+        <v>174</v>
+      </c>
+      <c r="K26" t="s">
+        <v>180</v>
+      </c>
+      <c r="L26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-    </row>
-    <row r="27" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+    </row>
+    <row r="27" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>52</v>
       </c>
@@ -1564,19 +1972,32 @@
         <v>18</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>122</v>
+        <v>97</v>
+      </c>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="G27" s="16"/>
-      <c r="H27" s="4" t="s">
+      <c r="H27" t="s">
+        <v>159</v>
+      </c>
+      <c r="I27" t="s">
+        <v>169</v>
+      </c>
+      <c r="J27" t="s">
+        <v>175</v>
+      </c>
+      <c r="K27" t="s">
+        <v>181</v>
+      </c>
+      <c r="L27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-    </row>
-    <row r="28" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+    </row>
+    <row r="28" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>53</v>
       </c>
@@ -1587,19 +2008,32 @@
         <v>18</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>123</v>
+        <v>98</v>
+      </c>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="G28" s="16"/>
-      <c r="H28" s="4" t="s">
+      <c r="H28" t="s">
+        <v>160</v>
+      </c>
+      <c r="I28" t="s">
+        <v>170</v>
+      </c>
+      <c r="J28" t="s">
+        <v>176</v>
+      </c>
+      <c r="K28" t="s">
+        <v>182</v>
+      </c>
+      <c r="L28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-    </row>
-    <row r="29" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+    </row>
+    <row r="29" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>54</v>
       </c>
@@ -1610,19 +2044,32 @@
         <v>55</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>134</v>
+        <v>105</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="G29" s="17"/>
-      <c r="H29" s="12" t="s">
+      <c r="H29" t="s">
+        <v>161</v>
+      </c>
+      <c r="I29" t="s">
+        <v>171</v>
+      </c>
+      <c r="J29" t="s">
+        <v>177</v>
+      </c>
+      <c r="K29" t="s">
+        <v>183</v>
+      </c>
+      <c r="L29" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-    </row>
-    <row r="30" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+    </row>
+    <row r="30" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>56</v>
       </c>
@@ -1633,19 +2080,32 @@
         <v>57</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>137</v>
+        <v>106</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17" t="s">
+        <v>145</v>
       </c>
       <c r="G30" s="17"/>
-      <c r="H30" s="12" t="s">
+      <c r="H30" t="s">
+        <v>162</v>
+      </c>
+      <c r="I30" t="s">
+        <v>172</v>
+      </c>
+      <c r="J30" t="s">
+        <v>178</v>
+      </c>
+      <c r="K30" t="s">
+        <v>184</v>
+      </c>
+      <c r="L30" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-    </row>
-    <row r="31" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+    </row>
+    <row r="31" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>58</v>
       </c>
@@ -1656,19 +2116,32 @@
         <v>29</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>139</v>
+        <v>107</v>
+      </c>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17" t="s">
+        <v>146</v>
       </c>
       <c r="G31" s="17"/>
-      <c r="H31" s="4" t="s">
+      <c r="H31" t="s">
+        <v>163</v>
+      </c>
+      <c r="I31" t="s">
+        <v>173</v>
+      </c>
+      <c r="J31" t="s">
+        <v>179</v>
+      </c>
+      <c r="K31" t="s">
+        <v>185</v>
+      </c>
+      <c r="L31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-    </row>
-    <row r="32" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+    </row>
+    <row r="32" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>59</v>
       </c>
@@ -1679,19 +2152,32 @@
         <v>60</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>133</v>
+        <v>103</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="G32" s="17"/>
-      <c r="H32" s="12" t="s">
+      <c r="H32" t="s">
+        <v>158</v>
+      </c>
+      <c r="I32" t="s">
+        <v>168</v>
+      </c>
+      <c r="J32" t="s">
+        <v>174</v>
+      </c>
+      <c r="K32" t="s">
+        <v>180</v>
+      </c>
+      <c r="L32" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-    </row>
-    <row r="33" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+    </row>
+    <row r="33" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>61</v>
       </c>
@@ -1702,19 +2188,32 @@
         <v>62</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>131</v>
+        <v>104</v>
+      </c>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="G33" s="17"/>
-      <c r="H33" s="12" t="s">
+      <c r="H33" t="s">
+        <v>159</v>
+      </c>
+      <c r="I33" t="s">
+        <v>169</v>
+      </c>
+      <c r="J33" t="s">
+        <v>175</v>
+      </c>
+      <c r="K33" t="s">
+        <v>181</v>
+      </c>
+      <c r="L33" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
         <v>63</v>
       </c>
@@ -1725,24 +2224,32 @@
         <v>30</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>128</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E34" s="17"/>
       <c r="F34" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="H34" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" s="17"/>
+      <c r="H34" t="s">
+        <v>160</v>
+      </c>
+      <c r="I34" t="s">
+        <v>170</v>
+      </c>
+      <c r="J34" t="s">
+        <v>176</v>
+      </c>
+      <c r="K34" t="s">
+        <v>182</v>
+      </c>
+      <c r="L34" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
         <v>64</v>
       </c>
@@ -1753,24 +2260,32 @@
         <v>30</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>129</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E35" s="17"/>
       <c r="F35" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="H35" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35" s="17"/>
+      <c r="H35" t="s">
+        <v>161</v>
+      </c>
+      <c r="I35" t="s">
+        <v>171</v>
+      </c>
+      <c r="J35" t="s">
+        <v>177</v>
+      </c>
+      <c r="K35" t="s">
+        <v>183</v>
+      </c>
+      <c r="L35" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>65</v>
       </c>
@@ -1781,16 +2296,28 @@
         <v>18</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="H36" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="H36" t="s">
+        <v>162</v>
+      </c>
+      <c r="I36" t="s">
+        <v>172</v>
+      </c>
+      <c r="J36" t="s">
+        <v>178</v>
+      </c>
+      <c r="K36" t="s">
+        <v>184</v>
+      </c>
+      <c r="L36" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>66</v>
       </c>
@@ -1801,17 +2328,30 @@
         <v>18</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>148</v>
+        <v>110</v>
+      </c>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18" t="s">
+        <v>149</v>
       </c>
       <c r="G37" s="18"/>
-      <c r="H37" s="15" t="s">
+      <c r="H37" t="s">
+        <v>163</v>
+      </c>
+      <c r="I37" t="s">
+        <v>173</v>
+      </c>
+      <c r="J37" t="s">
+        <v>179</v>
+      </c>
+      <c r="K37" t="s">
+        <v>185</v>
+      </c>
+      <c r="L37" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>67</v>
       </c>
@@ -1822,17 +2362,29 @@
         <v>18</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="H38" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="H38" t="s">
+        <v>159</v>
+      </c>
+      <c r="I38" t="s">
+        <v>168</v>
+      </c>
+      <c r="J38" t="s">
+        <v>174</v>
+      </c>
+      <c r="K38" t="s">
+        <v>180</v>
+      </c>
+      <c r="L38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M38" s="5"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>68</v>
       </c>
@@ -1843,17 +2395,29 @@
         <v>18</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="H39" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="H39" t="s">
+        <v>160</v>
+      </c>
+      <c r="I39" t="s">
+        <v>169</v>
+      </c>
+      <c r="J39" t="s">
+        <v>175</v>
+      </c>
+      <c r="K39" t="s">
+        <v>181</v>
+      </c>
+      <c r="L39" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M39" s="5"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>69</v>
       </c>
@@ -1864,17 +2428,29 @@
         <v>18</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="H40" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="H40" t="s">
+        <v>161</v>
+      </c>
+      <c r="I40" t="s">
+        <v>170</v>
+      </c>
+      <c r="J40" t="s">
+        <v>176</v>
+      </c>
+      <c r="K40" t="s">
+        <v>182</v>
+      </c>
+      <c r="L40" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M40" s="5"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>70</v>
       </c>
@@ -1885,17 +2461,29 @@
         <v>18</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="H41" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="H41" t="s">
+        <v>162</v>
+      </c>
+      <c r="I41" t="s">
+        <v>171</v>
+      </c>
+      <c r="J41" t="s">
+        <v>177</v>
+      </c>
+      <c r="K41" t="s">
+        <v>183</v>
+      </c>
+      <c r="L41" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M41" s="5"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>71</v>
       </c>
@@ -1906,17 +2494,29 @@
         <v>18</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="H42" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="H42" t="s">
+        <v>163</v>
+      </c>
+      <c r="I42" t="s">
+        <v>172</v>
+      </c>
+      <c r="J42" t="s">
+        <v>178</v>
+      </c>
+      <c r="K42" t="s">
+        <v>184</v>
+      </c>
+      <c r="L42" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="5"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M42" s="5"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>72</v>
       </c>
@@ -1927,15 +2527,27 @@
         <v>24</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="E43" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="H43" t="s">
         <v>158</v>
       </c>
-      <c r="H43" s="7" t="s">
+      <c r="I43" t="s">
+        <v>173</v>
+      </c>
+      <c r="J43" t="s">
+        <v>179</v>
+      </c>
+      <c r="K43" t="s">
+        <v>185</v>
+      </c>
+      <c r="L43" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="M43" s="5" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(excel-to-json): allow comments in class and property definitions (#111)
* Updating code to handle rdfs:comments in 4 languages in classe and property definition

* Updating Excel examples to handle rdfs:comment in 4 languages

* chore: add dependencies for python 3.10 compatibility

* refactor: minor code changes

* docs: update tooling documentation

* docs: update documentation according to changes, add excel template files

* chore: remove vars.mk

* refactor: remove code smell

* refactor: reduce code smell

* test: add unit test for creating resources from excel
</commit_message>
<xml_diff>
--- a/testdata/Properties.xlsx
+++ b/testdata/Properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ritagautschy/Documents/Ontologien/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrivoal/Git-projets/medialitterature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FCE124-D34B-FA49-A5DE-60DA442D292B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B05C1F0-00BF-A041-B1F2-B0672A71AD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="7320" windowWidth="24580" windowHeight="12560" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
+    <workbookView xWindow="15420" yWindow="4640" windowWidth="35780" windowHeight="23420" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="186">
   <si>
     <t>super</t>
   </si>
@@ -258,250 +258,331 @@
     <t>fr</t>
   </si>
   <si>
+    <t>owner of</t>
+  </si>
+  <si>
+    <t>anthroponym</t>
+  </si>
+  <si>
+    <t>generic anthroponym</t>
+  </si>
+  <si>
+    <t>designated as</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>related with</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>birth date</t>
+  </si>
+  <si>
+    <t>death date</t>
+  </si>
+  <si>
+    <t>bibliography</t>
+  </si>
+  <si>
+    <t>remark</t>
+  </si>
+  <si>
+    <t>corresponds to generic anthroponym</t>
+  </si>
+  <si>
+    <t>TM name identifier</t>
+  </si>
+  <si>
+    <t>Egyptian name</t>
+  </si>
+  <si>
+    <t>Greek name</t>
+  </si>
+  <si>
+    <t>Latin name</t>
+  </si>
+  <si>
+    <t>Coptic name</t>
+  </si>
+  <si>
+    <t>other name variant</t>
+  </si>
+  <si>
+    <t>linguistic origin</t>
+  </si>
+  <si>
+    <t>English translation</t>
+  </si>
+  <si>
+    <t>French translation</t>
+  </si>
+  <si>
+    <t>German translation</t>
+  </si>
+  <si>
+    <t>family relation</t>
+  </si>
+  <si>
+    <t>related to</t>
+  </si>
+  <si>
+    <t>terminus post quem</t>
+  </si>
+  <si>
+    <t>terminus ante quem</t>
+  </si>
+  <si>
+    <t>most common in</t>
+  </si>
+  <si>
+    <t>most widespread in</t>
+  </si>
+  <si>
+    <t>related to god</t>
+  </si>
+  <si>
+    <t>related to place</t>
+  </si>
+  <si>
+    <t>attested amount</t>
+  </si>
+  <si>
+    <t>has alias</t>
+  </si>
+  <si>
+    <t>is alias</t>
+  </si>
+  <si>
+    <t>is alais of</t>
+  </si>
+  <si>
+    <t>has title</t>
+  </si>
+  <si>
+    <t>English title</t>
+  </si>
+  <si>
+    <t>French title</t>
+  </si>
+  <si>
+    <t>German title</t>
+  </si>
+  <si>
+    <t>is equivalent to</t>
+  </si>
+  <si>
+    <t>occupation field</t>
+  </si>
+  <si>
+    <t>Anthroponyme</t>
+  </si>
+  <si>
+    <t>Propriétaire de</t>
+  </si>
+  <si>
+    <t>correspond à l'anthroponyme générique</t>
+  </si>
+  <si>
+    <t>a un alias</t>
+  </si>
+  <si>
+    <t>Genre</t>
+  </si>
+  <si>
+    <t>désigné sous le nom de</t>
+  </si>
+  <si>
+    <t>a un titre</t>
+  </si>
+  <si>
+    <t>statut</t>
+  </si>
+  <si>
+    <t>en rapport avec</t>
+  </si>
+  <si>
+    <t>Âge</t>
+  </si>
+  <si>
+    <t>Date de naissance</t>
+  </si>
+  <si>
+    <t>Date du décès</t>
+  </si>
+  <si>
+    <t>Littérature</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
+  </si>
+  <si>
+    <t>connecté avec</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Anthroponyme générique</t>
+  </si>
+  <si>
+    <t>Identifiant du nom de la MT</t>
+  </si>
+  <si>
+    <t>Nom égyptien</t>
+  </si>
+  <si>
+    <t>Nom grec</t>
+  </si>
+  <si>
+    <t>Nom latin</t>
+  </si>
+  <si>
+    <t>Nom copte</t>
+  </si>
+  <si>
+    <t>Autre variante du nom</t>
+  </si>
+  <si>
+    <t>origine linguistique</t>
+  </si>
+  <si>
+    <t>Traduction en anglais</t>
+  </si>
+  <si>
+    <t>Traduction en français</t>
+  </si>
+  <si>
+    <t>Traduction en allemand</t>
+  </si>
+  <si>
+    <t>associé à une divinité</t>
+  </si>
+  <si>
+    <t>associé à un lieu</t>
+  </si>
+  <si>
+    <t>Nombre de références</t>
+  </si>
+  <si>
+    <t>le plus courant dans</t>
+  </si>
+  <si>
+    <t>est un alias</t>
+  </si>
+  <si>
+    <t>est un alias de</t>
+  </si>
+  <si>
+    <t>titre</t>
+  </si>
+  <si>
+    <t>Titre anglais</t>
+  </si>
+  <si>
+    <t>Titre français</t>
+  </si>
+  <si>
+    <t>Titre allemand</t>
+  </si>
+  <si>
+    <t>est équivalent à</t>
+  </si>
+  <si>
+    <t>Domaine d'emploi</t>
+  </si>
+  <si>
+    <t>comment_fr</t>
+  </si>
+  <si>
+    <t>comment_en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A strange chance put me in possession of this journal.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I had established myself for several months in a central city in one of our southern departments, whose shore is bathed by the Mediterranean, and I was desirous of purchasing a country place in that marvellously picturesque land. </t>
+  </si>
+  <si>
+    <t>I had already looked at several pieces of property when, one day, the notary, who had been giving me some necessary directions for one of my explorations, said to me:</t>
+  </si>
+  <si>
+    <t>I have just received notice that at about eight leagues from here, in one of the most beautiful situations in the world, neither too far nor too near to the sea, there is a country house for sale.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I know nothing of it whatever; but if you would like to see it, monsieur, here are the precise directions how to find it. </t>
+  </si>
+  <si>
+    <t>You will have to arrange the affair with the curé of the village of ——."</t>
+  </si>
+  <si>
     <t>de</t>
   </si>
   <si>
-    <t>Anthroponym</t>
-  </si>
-  <si>
-    <t>Besitzer von</t>
-  </si>
-  <si>
-    <t>owner of</t>
-  </si>
-  <si>
-    <t>anthroponym</t>
-  </si>
-  <si>
-    <t>generic anthroponym</t>
-  </si>
-  <si>
-    <t>Generisches Anthroponym</t>
-  </si>
-  <si>
-    <t>Geschlecht</t>
-  </si>
-  <si>
-    <t>bezeichnet als</t>
-  </si>
-  <si>
-    <t>designated as</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>Titel</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>verwandt mit</t>
-  </si>
-  <si>
-    <t>related with</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>Alter</t>
-  </si>
-  <si>
-    <t>birth date</t>
-  </si>
-  <si>
-    <t>Geburtsdatum</t>
-  </si>
-  <si>
-    <t>death date</t>
-  </si>
-  <si>
-    <t>Sterbedatum</t>
-  </si>
-  <si>
-    <t>bibliography</t>
-  </si>
-  <si>
-    <t>Literatur</t>
-  </si>
-  <si>
-    <t>remark</t>
-  </si>
-  <si>
-    <t>Bemerkung</t>
-  </si>
-  <si>
-    <t>entspricht generischem Anthroponym</t>
-  </si>
-  <si>
-    <t>corresponds to generic anthroponym</t>
-  </si>
-  <si>
-    <t>TM name identifier</t>
-  </si>
-  <si>
-    <t>TM-Namensidentifikator</t>
-  </si>
-  <si>
-    <t>ägyptischer Name</t>
-  </si>
-  <si>
-    <t>griechischer Name</t>
-  </si>
-  <si>
-    <t>lateinischer Name</t>
-  </si>
-  <si>
-    <t>Egyptian name</t>
-  </si>
-  <si>
-    <t>Greek name</t>
-  </si>
-  <si>
-    <t>Latin name</t>
-  </si>
-  <si>
-    <t>Coptic name</t>
-  </si>
-  <si>
-    <t>Andere Namensvariante</t>
-  </si>
-  <si>
-    <t>koptischer Name</t>
-  </si>
-  <si>
-    <t>other name variant</t>
-  </si>
-  <si>
-    <t>linguistic origin</t>
-  </si>
-  <si>
-    <t>sprachlicher Ursprung</t>
-  </si>
-  <si>
-    <t>English translation</t>
-  </si>
-  <si>
-    <t>French translation</t>
-  </si>
-  <si>
-    <t>German translation</t>
-  </si>
-  <si>
-    <t>englische Übersetzung</t>
-  </si>
-  <si>
-    <t>französische Übersetzung</t>
-  </si>
-  <si>
-    <t>deutsche Übersetzung</t>
-  </si>
-  <si>
-    <t>Verwandtschaftsbeziehung</t>
-  </si>
-  <si>
-    <t>family relation</t>
-  </si>
-  <si>
-    <t>related to</t>
-  </si>
-  <si>
-    <t>verbunden mit</t>
-  </si>
-  <si>
-    <t>terminus post quem</t>
-  </si>
-  <si>
-    <t>terminus ante quem</t>
-  </si>
-  <si>
-    <t>most common in</t>
-  </si>
-  <si>
-    <t>am weitesten verbreitet in</t>
-  </si>
-  <si>
-    <t>most widespread in</t>
-  </si>
-  <si>
-    <t>am gebräuchlichsten in</t>
-  </si>
-  <si>
-    <t>verbunden mit Gottheit</t>
-  </si>
-  <si>
-    <t>related to god</t>
-  </si>
-  <si>
-    <t>related to place</t>
-  </si>
-  <si>
-    <t>verbunden mit Ort</t>
-  </si>
-  <si>
-    <t>attested amount</t>
-  </si>
-  <si>
-    <t>Anzahl Belegstellen</t>
-  </si>
-  <si>
     <t>it</t>
   </si>
   <si>
-    <t>has alias</t>
-  </si>
-  <si>
-    <t>hat Alias</t>
-  </si>
-  <si>
-    <t>is alias</t>
-  </si>
-  <si>
-    <t>ist Alias</t>
-  </si>
-  <si>
-    <t>is alais of</t>
-  </si>
-  <si>
-    <t>has title</t>
-  </si>
-  <si>
-    <t>hat Titel</t>
-  </si>
-  <si>
-    <t>ist Alias von</t>
-  </si>
-  <si>
-    <t>English title</t>
-  </si>
-  <si>
-    <t>French title</t>
-  </si>
-  <si>
-    <t>German title</t>
-  </si>
-  <si>
-    <t>englischer Titel</t>
-  </si>
-  <si>
-    <t>französischer Titel</t>
-  </si>
-  <si>
-    <t>deutscher Titel</t>
-  </si>
-  <si>
-    <t>is equivalent to</t>
-  </si>
-  <si>
-    <t>ist äquivalent zu</t>
-  </si>
-  <si>
-    <t>occupation field</t>
-  </si>
-  <si>
-    <t>Beschäftigungsfeld</t>
+    <t>comment_it</t>
+  </si>
+  <si>
+    <t>comment_de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein seltsamer Zufall brachte mich in den Besitz dieses Tagebuchs.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich hatte mich für einige Monate in einer Stadt im Zentrum eines unserer südlichen Departements niedergelassen, dessen Ufer vom Mittelmeer umspült wird, und wollte ein Grundstück in diesem wunderbar malerischen Land erwerben. </t>
+  </si>
+  <si>
+    <t>Ich hatte bereits mehrere Grundstücke besichtigt, als eines Tages der Notar, der mir die notwendigen Anweisungen für eine meiner Erkundungen gegeben hatte, zu mir sagte:</t>
+  </si>
+  <si>
+    <t>Ich habe soeben erfahren, dass etwa acht Meilen von hier, in einer der schönsten Lagen der Welt, weder zu weit noch zu nah am Meer, ein Landhaus zum Verkauf steht.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich weiß nichts davon, aber wenn Sie es sehen möchten, Monsieur, finden Sie hier die genaue Wegbeschreibung. </t>
+  </si>
+  <si>
+    <t>Sie werden die Angelegenheit mit dem Pfarrer des Dorfes -- regeln müssen."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un étrange hasard m'a mis en possession de ce journal.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je m'étais établi depuis plusieurs mois dans une ville centrale d'un de nos départements méridionaux, dont le rivage est baigné par la Méditerranée, et je désirais acheter une maison de campagne dans cette contrée merveilleusement pittoresque. </t>
+  </si>
+  <si>
+    <t>J'avais déjà examiné plusieurs propriétés quand, un jour, le notaire, qui me donnait des indications nécessaires pour une de mes explorations, me dit :</t>
+  </si>
+  <si>
+    <t>Je viens de recevoir avis qu'à huit lieues d'ici environ, dans une des plus belles situations du monde, ni trop loin ni trop près de la mer, il y a une maison de campagne à vendre.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je n'en sais rien du tout ; mais si vous voulez la voir, monsieur, voici les indications précises pour la trouver. </t>
+  </si>
+  <si>
+    <t>Vous devrez arranger l'affaire avec le curé du village de --."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uno strano caso mi mise in possesso di questo diario.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mi ero stabilito da diversi mesi in una città centrale di uno dei nostri dipartimenti del sud, la cui riva è bagnata dal Mediterraneo, e desideravo acquistare un posto in campagna in quella terra meravigliosamente pittoresca. </t>
+  </si>
+  <si>
+    <t>Avevo già visto diverse proprietà quando un giorno il notaio, che mi aveva dato alcune indicazioni necessarie per una delle mie esplorazioni, mi disse</t>
+  </si>
+  <si>
+    <t>Ho appena ricevuto la notizia che a circa otto leghe da qui, in una delle situazioni più belle del mondo, né troppo lontano né troppo vicino al mare, c'è una casa di campagna in vendita.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non ne so nulla; ma se volete vederla, signore, eccovi le indicazioni precise per trovarla. </t>
+  </si>
+  <si>
+    <t>Dovrete organizzare l'affare con il curato del villaggio di --".</t>
   </si>
 </sst>
 </file>
@@ -642,8 +723,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Feuil1" xfId="1" xr:uid="{62E45FE5-1366-448C-9556-6A8FC585BB6F}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -659,7 +740,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -955,11 +1036,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3015D75-1C5B-4AD1-9C97-0CD088290370}">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -967,19 +1048,21 @@
     <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="24" style="16" customWidth="1"/>
-    <col min="6" max="6" width="31.83203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="23.1640625" customWidth="1"/>
-    <col min="9" max="9" width="23.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="23.1640625" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="31.33203125" style="16" customWidth="1"/>
+    <col min="6" max="7" width="24" style="16" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" style="16" customWidth="1"/>
+    <col min="9" max="9" width="31.83203125" style="16" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" style="16" customWidth="1"/>
+    <col min="11" max="11" width="31.83203125" style="16" customWidth="1"/>
+    <col min="12" max="12" width="23.1640625" customWidth="1"/>
+    <col min="13" max="13" width="23.1640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="23.1640625" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="20" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>74</v>
       </c>
@@ -993,22 +1076,34 @@
         <v>75</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>77</v>
+        <v>164</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>76</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="H1" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="L1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1019,18 +1114,31 @@
         <v>18</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="16" t="s">
         <v>78</v>
       </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16" t="s">
+        <v>117</v>
+      </c>
       <c r="G2" s="16"/>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" t="s">
+        <v>168</v>
+      </c>
+      <c r="J2" t="s">
+        <v>174</v>
+      </c>
+      <c r="K2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -1041,18 +1149,31 @@
         <v>21</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="G3" s="16"/>
-      <c r="H3" s="8" t="s">
+      <c r="H3" t="s">
+        <v>159</v>
+      </c>
+      <c r="I3" t="s">
+        <v>169</v>
+      </c>
+      <c r="J3" t="s">
+        <v>175</v>
+      </c>
+      <c r="K3" t="s">
+        <v>181</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -1063,18 +1184,31 @@
         <v>38</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>102</v>
+        <v>88</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16" t="s">
+        <v>119</v>
       </c>
       <c r="G4" s="16"/>
-      <c r="H4" s="8" t="s">
+      <c r="H4" t="s">
+        <v>160</v>
+      </c>
+      <c r="I4" t="s">
+        <v>170</v>
+      </c>
+      <c r="J4" t="s">
+        <v>176</v>
+      </c>
+      <c r="K4" t="s">
+        <v>182</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M4" s="5"/>
+    </row>
+    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1085,18 +1219,31 @@
         <v>39</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>142</v>
+        <v>108</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16" t="s">
+        <v>120</v>
       </c>
       <c r="G5" s="16"/>
-      <c r="H5" s="8" t="s">
+      <c r="H5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I5" t="s">
+        <v>171</v>
+      </c>
+      <c r="J5" t="s">
+        <v>177</v>
+      </c>
+      <c r="K5" t="s">
+        <v>183</v>
+      </c>
+      <c r="L5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1109,18 +1256,31 @@
       <c r="D6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>84</v>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16" t="s">
+        <v>121</v>
       </c>
       <c r="G6" s="16"/>
-      <c r="H6" s="2" t="s">
+      <c r="H6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" t="s">
+        <v>172</v>
+      </c>
+      <c r="J6" t="s">
+        <v>178</v>
+      </c>
+      <c r="K6" t="s">
+        <v>184</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1131,20 +1291,33 @@
         <v>24</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>85</v>
+        <v>80</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16" t="s">
+        <v>122</v>
       </c>
       <c r="G7" s="16"/>
-      <c r="H7" s="7" t="s">
+      <c r="H7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I7" t="s">
+        <v>173</v>
+      </c>
+      <c r="J7" t="s">
+        <v>179</v>
+      </c>
+      <c r="K7" t="s">
+        <v>185</v>
+      </c>
+      <c r="L7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="M7" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1155,18 +1328,31 @@
         <v>40</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>147</v>
+        <v>111</v>
+      </c>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16" t="s">
+        <v>123</v>
       </c>
       <c r="G8" s="16"/>
-      <c r="H8" s="8" t="s">
+      <c r="H8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I8" t="s">
+        <v>168</v>
+      </c>
+      <c r="J8" t="s">
+        <v>174</v>
+      </c>
+      <c r="K8" t="s">
+        <v>180</v>
+      </c>
+      <c r="L8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1179,18 +1365,31 @@
       <c r="D9" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>89</v>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="G9" s="16"/>
-      <c r="H9" s="7" t="s">
+      <c r="H9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I9" t="s">
+        <v>169</v>
+      </c>
+      <c r="J9" t="s">
+        <v>175</v>
+      </c>
+      <c r="K9" t="s">
+        <v>181</v>
+      </c>
+      <c r="L9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="M9" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1201,18 +1400,31 @@
         <v>41</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>90</v>
+        <v>82</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16" t="s">
+        <v>125</v>
       </c>
       <c r="G10" s="16"/>
-      <c r="H10" s="8" t="s">
+      <c r="H10" t="s">
+        <v>160</v>
+      </c>
+      <c r="I10" t="s">
+        <v>170</v>
+      </c>
+      <c r="J10" t="s">
+        <v>176</v>
+      </c>
+      <c r="K10" t="s">
+        <v>182</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1223,18 +1435,31 @@
         <v>29</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>93</v>
+        <v>83</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="G11" s="16"/>
-      <c r="H11" s="7" t="s">
+      <c r="H11" t="s">
+        <v>161</v>
+      </c>
+      <c r="I11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1245,16 +1470,28 @@
         <v>30</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="H12" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" t="s">
+        <v>162</v>
+      </c>
+      <c r="I12" t="s">
+        <v>172</v>
+      </c>
+      <c r="J12" t="s">
+        <v>178</v>
+      </c>
+      <c r="K12" t="s">
+        <v>184</v>
+      </c>
+      <c r="L12" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1265,16 +1502,28 @@
         <v>30</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="H13" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" t="s">
+        <v>163</v>
+      </c>
+      <c r="I13" t="s">
+        <v>173</v>
+      </c>
+      <c r="J13" t="s">
+        <v>179</v>
+      </c>
+      <c r="K13" t="s">
+        <v>185</v>
+      </c>
+      <c r="L13" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -1285,16 +1534,28 @@
         <v>32</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="H14" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H14" t="s">
+        <v>158</v>
+      </c>
+      <c r="I14" t="s">
+        <v>168</v>
+      </c>
+      <c r="J14" t="s">
+        <v>174</v>
+      </c>
+      <c r="K14" t="s">
+        <v>180</v>
+      </c>
+      <c r="L14" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1305,16 +1566,28 @@
         <v>18</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="H15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="H15" t="s">
+        <v>159</v>
+      </c>
+      <c r="I15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J15" t="s">
+        <v>175</v>
+      </c>
+      <c r="K15" t="s">
+        <v>181</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>34</v>
       </c>
@@ -1325,17 +1598,29 @@
         <v>35</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="H16" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="H16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I16" t="s">
+        <v>170</v>
+      </c>
+      <c r="J16" t="s">
+        <v>176</v>
+      </c>
+      <c r="K16" t="s">
+        <v>182</v>
+      </c>
+      <c r="L16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -1346,19 +1631,31 @@
         <v>24</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="H17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="H17" t="s">
+        <v>161</v>
+      </c>
+      <c r="I17" t="s">
+        <v>171</v>
+      </c>
+      <c r="J17" t="s">
+        <v>177</v>
+      </c>
+      <c r="K17" t="s">
+        <v>183</v>
+      </c>
+      <c r="L17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="M17" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
@@ -1369,18 +1666,31 @@
         <v>18</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16" t="s">
+        <v>133</v>
       </c>
       <c r="G18" s="16"/>
-      <c r="H18" s="4" t="s">
+      <c r="H18" t="s">
+        <v>162</v>
+      </c>
+      <c r="I18" t="s">
+        <v>172</v>
+      </c>
+      <c r="J18" t="s">
+        <v>178</v>
+      </c>
+      <c r="K18" t="s">
+        <v>184</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O18" s="4"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -1391,17 +1701,29 @@
         <v>29</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="H19" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" t="s">
+        <v>163</v>
+      </c>
+      <c r="I19" t="s">
+        <v>173</v>
+      </c>
+      <c r="J19" t="s">
+        <v>179</v>
+      </c>
+      <c r="K19" t="s">
+        <v>185</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -1412,17 +1734,29 @@
         <v>18</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>106</v>
+        <v>90</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>135</v>
       </c>
       <c r="H20" t="s">
+        <v>158</v>
+      </c>
+      <c r="I20" t="s">
+        <v>168</v>
+      </c>
+      <c r="J20" t="s">
+        <v>174</v>
+      </c>
+      <c r="K20" t="s">
+        <v>180</v>
+      </c>
+      <c r="L20" t="s">
         <v>19</v>
       </c>
-      <c r="I20"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M20"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1433,17 +1767,29 @@
         <v>18</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>107</v>
+        <v>91</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>136</v>
       </c>
       <c r="H21" t="s">
+        <v>159</v>
+      </c>
+      <c r="I21" t="s">
+        <v>169</v>
+      </c>
+      <c r="J21" t="s">
+        <v>175</v>
+      </c>
+      <c r="K21" t="s">
+        <v>181</v>
+      </c>
+      <c r="L21" t="s">
         <v>19</v>
       </c>
-      <c r="I21"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M21"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1454,17 +1800,29 @@
         <v>18</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>108</v>
-      </c>
-      <c r="H22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" t="s">
+        <v>160</v>
+      </c>
+      <c r="I22" t="s">
+        <v>170</v>
+      </c>
+      <c r="J22" t="s">
+        <v>176</v>
+      </c>
+      <c r="K22" t="s">
+        <v>182</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I22"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M22"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1475,17 +1833,29 @@
         <v>18</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>114</v>
+        <v>93</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>138</v>
       </c>
       <c r="H23" t="s">
+        <v>161</v>
+      </c>
+      <c r="I23" t="s">
+        <v>171</v>
+      </c>
+      <c r="J23" t="s">
+        <v>177</v>
+      </c>
+      <c r="K23" t="s">
+        <v>183</v>
+      </c>
+      <c r="L23" t="s">
         <v>19</v>
       </c>
-      <c r="I23"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M23"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1496,17 +1866,29 @@
         <v>18</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="H24" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="H24" t="s">
+        <v>162</v>
+      </c>
+      <c r="I24" t="s">
+        <v>172</v>
+      </c>
+      <c r="J24" t="s">
+        <v>178</v>
+      </c>
+      <c r="K24" t="s">
+        <v>184</v>
+      </c>
+      <c r="L24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I24"/>
-    </row>
-    <row r="25" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M24"/>
+    </row>
+    <row r="25" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
@@ -1517,20 +1899,33 @@
         <v>24</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>117</v>
+        <v>95</v>
+      </c>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="G25" s="16"/>
-      <c r="H25" s="2" t="s">
+      <c r="H25" t="s">
+        <v>163</v>
+      </c>
+      <c r="I25" t="s">
+        <v>173</v>
+      </c>
+      <c r="J25" t="s">
+        <v>179</v>
+      </c>
+      <c r="K25" t="s">
+        <v>185</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="M25" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>51</v>
       </c>
@@ -1541,19 +1936,32 @@
         <v>18</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>121</v>
+        <v>96</v>
+      </c>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="G26" s="16"/>
-      <c r="H26" s="4" t="s">
+      <c r="H26" t="s">
+        <v>158</v>
+      </c>
+      <c r="I26" t="s">
+        <v>168</v>
+      </c>
+      <c r="J26" t="s">
+        <v>174</v>
+      </c>
+      <c r="K26" t="s">
+        <v>180</v>
+      </c>
+      <c r="L26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-    </row>
-    <row r="27" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+    </row>
+    <row r="27" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>52</v>
       </c>
@@ -1564,19 +1972,32 @@
         <v>18</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>122</v>
+        <v>97</v>
+      </c>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="G27" s="16"/>
-      <c r="H27" s="4" t="s">
+      <c r="H27" t="s">
+        <v>159</v>
+      </c>
+      <c r="I27" t="s">
+        <v>169</v>
+      </c>
+      <c r="J27" t="s">
+        <v>175</v>
+      </c>
+      <c r="K27" t="s">
+        <v>181</v>
+      </c>
+      <c r="L27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-    </row>
-    <row r="28" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+    </row>
+    <row r="28" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>53</v>
       </c>
@@ -1587,19 +2008,32 @@
         <v>18</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>123</v>
+        <v>98</v>
+      </c>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="G28" s="16"/>
-      <c r="H28" s="4" t="s">
+      <c r="H28" t="s">
+        <v>160</v>
+      </c>
+      <c r="I28" t="s">
+        <v>170</v>
+      </c>
+      <c r="J28" t="s">
+        <v>176</v>
+      </c>
+      <c r="K28" t="s">
+        <v>182</v>
+      </c>
+      <c r="L28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-    </row>
-    <row r="29" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+    </row>
+    <row r="29" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>54</v>
       </c>
@@ -1610,19 +2044,32 @@
         <v>55</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>134</v>
+        <v>105</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17" t="s">
+        <v>144</v>
       </c>
       <c r="G29" s="17"/>
-      <c r="H29" s="12" t="s">
+      <c r="H29" t="s">
+        <v>161</v>
+      </c>
+      <c r="I29" t="s">
+        <v>171</v>
+      </c>
+      <c r="J29" t="s">
+        <v>177</v>
+      </c>
+      <c r="K29" t="s">
+        <v>183</v>
+      </c>
+      <c r="L29" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-    </row>
-    <row r="30" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+    </row>
+    <row r="30" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>56</v>
       </c>
@@ -1633,19 +2080,32 @@
         <v>57</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>137</v>
+        <v>106</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17" t="s">
+        <v>145</v>
       </c>
       <c r="G30" s="17"/>
-      <c r="H30" s="12" t="s">
+      <c r="H30" t="s">
+        <v>162</v>
+      </c>
+      <c r="I30" t="s">
+        <v>172</v>
+      </c>
+      <c r="J30" t="s">
+        <v>178</v>
+      </c>
+      <c r="K30" t="s">
+        <v>184</v>
+      </c>
+      <c r="L30" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-    </row>
-    <row r="31" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+    </row>
+    <row r="31" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>58</v>
       </c>
@@ -1656,19 +2116,32 @@
         <v>29</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>139</v>
+        <v>107</v>
+      </c>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17" t="s">
+        <v>146</v>
       </c>
       <c r="G31" s="17"/>
-      <c r="H31" s="4" t="s">
+      <c r="H31" t="s">
+        <v>163</v>
+      </c>
+      <c r="I31" t="s">
+        <v>173</v>
+      </c>
+      <c r="J31" t="s">
+        <v>179</v>
+      </c>
+      <c r="K31" t="s">
+        <v>185</v>
+      </c>
+      <c r="L31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-    </row>
-    <row r="32" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+    </row>
+    <row r="32" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>59</v>
       </c>
@@ -1679,19 +2152,32 @@
         <v>60</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>133</v>
+        <v>103</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="G32" s="17"/>
-      <c r="H32" s="12" t="s">
+      <c r="H32" t="s">
+        <v>158</v>
+      </c>
+      <c r="I32" t="s">
+        <v>168</v>
+      </c>
+      <c r="J32" t="s">
+        <v>174</v>
+      </c>
+      <c r="K32" t="s">
+        <v>180</v>
+      </c>
+      <c r="L32" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-    </row>
-    <row r="33" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+    </row>
+    <row r="33" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>61</v>
       </c>
@@ -1702,19 +2188,32 @@
         <v>62</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>131</v>
+        <v>104</v>
+      </c>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17" t="s">
+        <v>147</v>
       </c>
       <c r="G33" s="17"/>
-      <c r="H33" s="12" t="s">
+      <c r="H33" t="s">
+        <v>159</v>
+      </c>
+      <c r="I33" t="s">
+        <v>169</v>
+      </c>
+      <c r="J33" t="s">
+        <v>175</v>
+      </c>
+      <c r="K33" t="s">
+        <v>181</v>
+      </c>
+      <c r="L33" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
         <v>63</v>
       </c>
@@ -1725,24 +2224,32 @@
         <v>30</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>128</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E34" s="17"/>
       <c r="F34" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="H34" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" s="17"/>
+      <c r="H34" t="s">
+        <v>160</v>
+      </c>
+      <c r="I34" t="s">
+        <v>170</v>
+      </c>
+      <c r="J34" t="s">
+        <v>176</v>
+      </c>
+      <c r="K34" t="s">
+        <v>182</v>
+      </c>
+      <c r="L34" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
         <v>64</v>
       </c>
@@ -1753,24 +2260,32 @@
         <v>30</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>129</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E35" s="17"/>
       <c r="F35" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="H35" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35" s="17"/>
+      <c r="H35" t="s">
+        <v>161</v>
+      </c>
+      <c r="I35" t="s">
+        <v>171</v>
+      </c>
+      <c r="J35" t="s">
+        <v>177</v>
+      </c>
+      <c r="K35" t="s">
+        <v>183</v>
+      </c>
+      <c r="L35" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>65</v>
       </c>
@@ -1781,16 +2296,28 @@
         <v>18</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="H36" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="H36" t="s">
+        <v>162</v>
+      </c>
+      <c r="I36" t="s">
+        <v>172</v>
+      </c>
+      <c r="J36" t="s">
+        <v>178</v>
+      </c>
+      <c r="K36" t="s">
+        <v>184</v>
+      </c>
+      <c r="L36" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>66</v>
       </c>
@@ -1801,17 +2328,30 @@
         <v>18</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>148</v>
+        <v>110</v>
+      </c>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18" t="s">
+        <v>149</v>
       </c>
       <c r="G37" s="18"/>
-      <c r="H37" s="15" t="s">
+      <c r="H37" t="s">
+        <v>163</v>
+      </c>
+      <c r="I37" t="s">
+        <v>173</v>
+      </c>
+      <c r="J37" t="s">
+        <v>179</v>
+      </c>
+      <c r="K37" t="s">
+        <v>185</v>
+      </c>
+      <c r="L37" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>67</v>
       </c>
@@ -1822,17 +2362,29 @@
         <v>18</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="H38" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="H38" t="s">
+        <v>159</v>
+      </c>
+      <c r="I38" t="s">
+        <v>168</v>
+      </c>
+      <c r="J38" t="s">
+        <v>174</v>
+      </c>
+      <c r="K38" t="s">
+        <v>180</v>
+      </c>
+      <c r="L38" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M38" s="5"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>68</v>
       </c>
@@ -1843,17 +2395,29 @@
         <v>18</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="H39" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="H39" t="s">
+        <v>160</v>
+      </c>
+      <c r="I39" t="s">
+        <v>169</v>
+      </c>
+      <c r="J39" t="s">
+        <v>175</v>
+      </c>
+      <c r="K39" t="s">
+        <v>181</v>
+      </c>
+      <c r="L39" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M39" s="5"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>69</v>
       </c>
@@ -1864,17 +2428,29 @@
         <v>18</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="H40" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="H40" t="s">
+        <v>161</v>
+      </c>
+      <c r="I40" t="s">
+        <v>170</v>
+      </c>
+      <c r="J40" t="s">
+        <v>176</v>
+      </c>
+      <c r="K40" t="s">
+        <v>182</v>
+      </c>
+      <c r="L40" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M40" s="5"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>70</v>
       </c>
@@ -1885,17 +2461,29 @@
         <v>18</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="H41" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="H41" t="s">
+        <v>162</v>
+      </c>
+      <c r="I41" t="s">
+        <v>171</v>
+      </c>
+      <c r="J41" t="s">
+        <v>177</v>
+      </c>
+      <c r="K41" t="s">
+        <v>183</v>
+      </c>
+      <c r="L41" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M41" s="5"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>71</v>
       </c>
@@ -1906,17 +2494,29 @@
         <v>18</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="H42" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="H42" t="s">
+        <v>163</v>
+      </c>
+      <c r="I42" t="s">
+        <v>172</v>
+      </c>
+      <c r="J42" t="s">
+        <v>178</v>
+      </c>
+      <c r="K42" t="s">
+        <v>184</v>
+      </c>
+      <c r="L42" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="5"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M42" s="5"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>72</v>
       </c>
@@ -1927,15 +2527,27 @@
         <v>24</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="E43" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="H43" t="s">
         <v>158</v>
       </c>
-      <c r="H43" s="7" t="s">
+      <c r="I43" t="s">
+        <v>173</v>
+      </c>
+      <c r="J43" t="s">
+        <v>179</v>
+      </c>
+      <c r="K43" t="s">
+        <v>185</v>
+      </c>
+      <c r="L43" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="M43" s="5" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
unittests: check contents of outfile, not only if it exists testdata: include more cases
</commit_message>
<xml_diff>
--- a/testdata/Properties.xlsx
+++ b/testdata/Properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535428BE-A610-0C4F-8B53-BCA0FB2E52BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762BC181-7EBB-B94D-BD80-04DEB7E12D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="259">
   <si>
     <t>super</t>
   </si>
@@ -790,6 +790,18 @@
   </si>
   <si>
     <t>hlist: status</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>because</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> is </t>
+  </si>
+  <si>
+    <t>missing!</t>
   </si>
 </sst>
 </file>
@@ -1210,11 +1222,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3015D75-1C5B-4AD1-9C97-0CD088290370}">
-  <dimension ref="A1:Q58"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD8"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3129,42 +3141,129 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>249</v>
+        <v>255</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>257</v>
       </c>
       <c r="K55" s="7" t="s">
-        <v>249</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="L55" s="2"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="J56" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="L56" s="2" t="s">
-        <v>249</v>
+        <v>256</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="L56" s="7" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="J57" s="7" t="s">
-        <v>249</v>
+        <v>256</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="L57" s="7" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="L58" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="I58" s="7" t="s">
+      <c r="K62" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="J63" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="J64" s="7" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B65" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I65" s="7" t="s">
         <v>249</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(xmlupload): implement <annotation>, <region>, and <link> tags (DEV-855) (#204)
These tags correspond to the DSP base resources Annotation, Region, LinkObj
</commit_message>
<xml_diff>
--- a/testdata/Properties.xlsx
+++ b/testdata/Properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA6D2DA-7ECD-0145-8C2C-D9888715AA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA06421-B858-9B44-BA75-E0E71D2179D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="137">
   <si>
     <t>super</t>
   </si>
@@ -313,18 +313,6 @@
   </si>
   <si>
     <t>Colorpicker</t>
-  </si>
-  <si>
-    <t>hasGeometry</t>
-  </si>
-  <si>
-    <t>GeomValue</t>
-  </si>
-  <si>
-    <t>Geometric object</t>
-  </si>
-  <si>
-    <t>Geometrisches Objekt</t>
   </si>
   <si>
     <t>Radio</t>
@@ -853,11 +841,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3015D75-1C5B-4AD1-9C97-0CD088290370}">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -898,7 +886,7 @@
         <v>43</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>37</v>
@@ -913,17 +901,17 @@
         <v>44</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="P1"/>
       <c r="Q1" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -934,10 +922,10 @@
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -947,41 +935,41 @@
         <v>39</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="O2" s="9"/>
       <c r="P2" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -999,14 +987,14 @@
         <v>54</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="O3" s="9"/>
       <c r="Q3" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1022,7 +1010,7 @@
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1039,19 +1027,19 @@
         <v>55</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="O4" s="9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1068,7 +1056,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="1" t="s">
@@ -1084,22 +1072,22 @@
         <v>56</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="O5" s="9" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1117,7 +1105,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>38</v>
@@ -1132,17 +1120,17 @@
         <v>54</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="O6" s="9"/>
       <c r="P6" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1164,16 +1152,16 @@
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1195,11 +1183,11 @@
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1209,13 +1197,13 @@
       </c>
       <c r="O8" s="9"/>
       <c r="Q8" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1235,10 +1223,10 @@
         <v>34</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>21</v>
@@ -1247,468 +1235,450 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>130</v>
+        <v>100</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O10" s="10"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>135</v>
+        <v>30</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O11" s="10"/>
+        <v>70</v>
+      </c>
+      <c r="O11" s="9"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
+      <c r="A12" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>35</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="6"/>
       <c r="H12" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>112</v>
+        <v>39</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>112</v>
+        <v>47</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>112</v>
+        <v>51</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="O12" s="9"/>
+        <v>120</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" s="3"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>24</v>
+      <c r="A13" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="6"/>
+      <c r="C13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="H13" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>140</v>
+        <v>120</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O13" s="3"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" t="s">
-        <v>137</v>
+        <v>120</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>116</v>
+        <v>95</v>
+      </c>
+      <c r="O14" s="9"/>
+      <c r="Q14" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>94</v>
+        <v>66</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="O15" s="9"/>
-      <c r="Q15" t="s">
-        <v>138</v>
+        <v>66</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>114</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O16" s="9"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O17" s="9"/>
+        <v>82</v>
+      </c>
+      <c r="O17" s="10"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="O18" s="10"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="O19" s="10"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="O20" s="10"/>
+        <v>15</v>
+      </c>
+      <c r="P20" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P21" t="s">
-        <v>139</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="N21" s="1"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>2</v>
+        <v>115</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="N22" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>118</v>
+      <c r="B24" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="N25" s="5" t="s">
-        <v>121</v>
-      </c>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="N27" s="1"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
@@ -1723,50 +1693,44 @@
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="N30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L31" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add isSequenceOf (DEV-746) (#214)
</commit_message>
<xml_diff>
--- a/testdata/Properties.xlsx
+++ b/testdata/Properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA06421-B858-9B44-BA75-E0E71D2179D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F722F936-5C6C-F348-B75C-95BF5A23BC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="138">
   <si>
     <t>super</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t xml:space="preserve">Avevo già visto diverse proprietà quando un giorno il notaio, </t>
+  </si>
+  <si>
+    <t>hasSequenceBounds</t>
   </si>
 </sst>
 </file>
@@ -845,7 +848,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1500,7 +1503,7 @@
         <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>137</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>79</v>

</xml_diff>